<commit_message>
added values for flashcards
</commit_message>
<xml_diff>
--- a/EnglishQuestions.xlsx
+++ b/EnglishQuestions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phyllis/Desktop/chinatowncitizenship/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenni\Documents\GitHub\chinatowncitizenship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C73E79-B616-F84F-8D17-8ED6B7E604BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DFC55B-B215-444D-AF7E-E1244E6D9FA1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10810" yWindow="3310" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="248">
   <si>
     <t>2005年 11月 15号</t>
   </si>
@@ -439,16 +439,359 @@
   </si>
   <si>
     <t>I have lived here for a while</t>
+  </si>
+  <si>
+    <t>Twenty-third</t>
+  </si>
+  <si>
+    <t>二十七</t>
+  </si>
+  <si>
+    <t>第二十三</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>一月</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>三月</t>
+  </si>
+  <si>
+    <t>Birthday</t>
+  </si>
+  <si>
+    <t>出生日期</t>
+  </si>
+  <si>
+    <t>Anniversary</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Twenty-seven</t>
+  </si>
+  <si>
+    <t>Twenty-seventh</t>
+  </si>
+  <si>
+    <t>Twenty-three</t>
+  </si>
+  <si>
+    <t>Thirty-two</t>
+  </si>
+  <si>
+    <t>Thirty-second</t>
+  </si>
+  <si>
+    <t>四月</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Hair</t>
+  </si>
+  <si>
+    <t>Eyes</t>
+  </si>
+  <si>
+    <t>Children</t>
+  </si>
+  <si>
+    <t>孩子</t>
+  </si>
+  <si>
+    <t>眼睛</t>
+  </si>
+  <si>
+    <t>头发</t>
+  </si>
+  <si>
+    <t>黑色的</t>
+  </si>
+  <si>
+    <t>棕色的</t>
+  </si>
+  <si>
+    <t>耳朵</t>
+  </si>
+  <si>
+    <t>父母</t>
+  </si>
+  <si>
+    <t>孙子</t>
+  </si>
+  <si>
+    <t>Grandchildren</t>
+  </si>
+  <si>
+    <t>How tall are you?</t>
+  </si>
+  <si>
+    <t>I am 5 feet, 2 inches tall</t>
+  </si>
+  <si>
+    <t>I weigh 100 pounds</t>
+  </si>
+  <si>
+    <t>My eyes are brown.</t>
+  </si>
+  <si>
+    <t>My hair is white.</t>
+  </si>
+  <si>
+    <t>How many children do you have?</t>
+  </si>
+  <si>
+    <t>你有几个孩子</t>
+  </si>
+  <si>
+    <t>你有几个孙子</t>
+  </si>
+  <si>
+    <t>你有几个女儿</t>
+  </si>
+  <si>
+    <t>你有几个儿子</t>
+  </si>
+  <si>
+    <t>Foodstamp</t>
+  </si>
+  <si>
+    <t>食物票</t>
+  </si>
+  <si>
+    <t>Tax</t>
+  </si>
+  <si>
+    <t>税</t>
+  </si>
+  <si>
+    <t>Welfare</t>
+  </si>
+  <si>
+    <t>社会福利</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>积蓄</t>
+  </si>
+  <si>
+    <t>Job</t>
+  </si>
+  <si>
+    <t>工作</t>
+  </si>
+  <si>
+    <t>How do you support yourself?</t>
+  </si>
+  <si>
+    <t>My children support me.</t>
+  </si>
+  <si>
+    <t>I am on welfare.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I have a job.</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>I pay my taxes</t>
+  </si>
+  <si>
+    <t>Social Security Number</t>
+  </si>
+  <si>
+    <t>Permanent Resident</t>
+  </si>
+  <si>
+    <t>社会安全号码</t>
+  </si>
+  <si>
+    <t>永久居民</t>
+  </si>
+  <si>
+    <t>Vacation</t>
+  </si>
+  <si>
+    <t>旅游</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>家人</t>
+  </si>
+  <si>
+    <t>America</t>
+  </si>
+  <si>
+    <t>美国</t>
+  </si>
+  <si>
+    <t>中国</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>英国</t>
+  </si>
+  <si>
+    <t>England</t>
+  </si>
+  <si>
+    <t>加拿大</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>North America</t>
+  </si>
+  <si>
+    <t>北美</t>
+  </si>
+  <si>
+    <t>Do you miss anything about China?</t>
+  </si>
+  <si>
+    <t>I miss my family.</t>
+  </si>
+  <si>
+    <t>I miss the food.</t>
+  </si>
+  <si>
+    <t>No, I do not miss anything.</t>
+  </si>
+  <si>
+    <t>I like to travel</t>
+  </si>
+  <si>
+    <t>The air is good</t>
+  </si>
+  <si>
+    <t>I want to sponsor my family to come to America</t>
+  </si>
+  <si>
+    <t>Why do you want to be an American citizen?</t>
+  </si>
+  <si>
+    <t>To travel with a U.S. passport.</t>
+  </si>
+  <si>
+    <t>To obtain federal government jobs.</t>
+  </si>
+  <si>
+    <t>To get social security benefits.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> My son.</t>
+  </si>
+  <si>
+    <t>I have been a permanent resident for 8 years.</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>左</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>右</t>
+  </si>
+  <si>
+    <t>Corridor</t>
+  </si>
+  <si>
+    <t>走廊</t>
+  </si>
+  <si>
+    <t>Wait</t>
+  </si>
+  <si>
+    <t>Wrong</t>
+  </si>
+  <si>
+    <t>错了</t>
+  </si>
+  <si>
+    <t>表示考官没有听清楚你刚说的话所以想让你重复一遍.</t>
+  </si>
+  <si>
+    <t>Pardon</t>
+  </si>
+  <si>
+    <t>Excuse me?</t>
+  </si>
+  <si>
+    <t>Can you repeat that?</t>
+  </si>
+  <si>
+    <t>Can you translate that?</t>
+  </si>
+  <si>
+    <t>I do not understand</t>
+  </si>
+  <si>
+    <t>楼梯</t>
+  </si>
+  <si>
+    <t>走</t>
+  </si>
+  <si>
+    <t>对</t>
+  </si>
+  <si>
+    <t>做得好</t>
+  </si>
+  <si>
+    <t>电梯</t>
+  </si>
+  <si>
+    <t>站起来</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -474,9 +817,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -757,1252 +1109,1947 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G62" sqref="E60:G62"/>
+    <sheetView tabSelected="1" topLeftCell="H65" zoomScale="49" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="Q87" sqref="Q87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="4" width="39.5" style="1" customWidth="1"/>
-    <col min="5" max="8" width="39.5" customWidth="1"/>
+    <col min="1" max="1" width="23" style="3" customWidth="1"/>
+    <col min="2" max="2" width="39.453125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="30.1796875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="24.81640625" style="4" customWidth="1"/>
+    <col min="5" max="8" width="39.453125" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="8.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I1">
+      <c r="I1" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G27" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G29" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G30" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="H30" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G31" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F32" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G32" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H33" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F34" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G34" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="H34" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F35" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G35" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="H35" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="I35">
+      <c r="I35" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F36" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="G36" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="H36" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="I36">
+      <c r="I36" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F37" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="G37" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="H37" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="I37">
+      <c r="I37" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F38" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G38" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="H38" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="I38">
+      <c r="I38" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F39" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G39" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="H39" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F40" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="H40" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="I40">
+      <c r="I40" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F41" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G41" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H41" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F42" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G42" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="H42" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="I42">
+      <c r="I42" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F43" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G43" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="H43" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="I43">
+      <c r="I43" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A44" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="F44" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="G44" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="H44" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="I44">
+      <c r="I44" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A45" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C45"/>
-      <c r="D45"/>
-      <c r="E45" s="1" t="s">
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F45" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="G45" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="H45" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I45">
+      <c r="I45" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="G46" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="H46" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I46">
+      <c r="I46" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A47" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F47" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="G47" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="H47" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="I47">
+      <c r="I47" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A48" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="F48" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="G48" s="1" t="s">
+      <c r="G48" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="H48" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="I48">
+      <c r="I48" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="F49" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="G49" s="1" t="s">
+      <c r="G49" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="H49" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="I49">
+      <c r="I49" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A50" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="F50" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G50" s="1" t="s">
+      <c r="G50" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="H50" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="I50">
+      <c r="I50" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A51" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="H51" s="1"/>
-      <c r="I51">
+      <c r="H51" s="4"/>
+      <c r="I51" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E52" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="H52" s="1"/>
-      <c r="I52">
+      <c r="H52" s="4"/>
+      <c r="I52" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A53" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="F53" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="I53">
+      <c r="I53" s="3">
         <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A54" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="I54" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A55" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="I55" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A56" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="I56" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="I57" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A58" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="I58" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A59" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="I59" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A60" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="I60" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A61" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="I61" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A62" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="I62" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A63" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="I63" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A64" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I64" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A65" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="I65" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A66" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="I66" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A67" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="I67" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A68" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="I68" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A69" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="I69" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A70" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="I70" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A71" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G71" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="I71" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A72" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="G72" s="4"/>
+      <c r="I72" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A73" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="I73" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A74" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="I74" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A75" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="I75" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A76" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="I76" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A77" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="H77" s="4"/>
+      <c r="I77" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A78" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="H78" s="4"/>
+      <c r="I78" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A79" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="H79" s="4"/>
+      <c r="I79" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A80" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="H80" s="4"/>
+      <c r="I80" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A81" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="I81" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A82" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="G82" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="I82" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A83" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="G83" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="I83" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="18" x14ac:dyDescent="0.4">
+      <c r="A84" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="I84" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="18" x14ac:dyDescent="0.4">
+      <c r="A85" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="I85" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A86" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="I86" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A87" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="I87" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A88" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="I88" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A89" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="I89" s="3">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>